<commit_message>
updating 2021 data. verified
</commit_message>
<xml_diff>
--- a/citations/publisher_emerald_2021_counts.xlsx
+++ b/citations/publisher_emerald_2021_counts.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B121"/>
+  <dimension ref="A1:B116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -422,7 +422,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Aslib Journal of Information Management</t>
+          <t>Aslib Proceedings</t>
         </is>
       </c>
       <c r="B7">
@@ -432,67 +432,67 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Aslib Proceedings</t>
+          <t>British Food Journal</t>
         </is>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>British Food Journal</t>
+          <t>Contributions to economic analysis</t>
         </is>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Contributions to economic analysis</t>
+          <t>Data Technologies and Applications</t>
         </is>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Data Technologies and Applications</t>
+          <t>Disaster Prevention and Management An International Journal</t>
         </is>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Disaster Prevention and Management An International Journal</t>
+          <t>Education + Training</t>
         </is>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Education + Training</t>
+          <t>Employee Relations</t>
         </is>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Employee Relations</t>
+          <t>Engineering Computations</t>
         </is>
       </c>
       <c r="B14">
@@ -502,17 +502,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Engineering Computations</t>
+          <t>Environmental Management and Health</t>
         </is>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Environmental Management and Health</t>
+          <t>Equal Opportunities International</t>
         </is>
       </c>
       <c r="B16">
@@ -522,7 +522,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Equal Opportunities International</t>
+          <t>European Journal of Innovation Management</t>
         </is>
       </c>
       <c r="B17">
@@ -532,7 +532,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>European Journal of Innovation Management</t>
+          <t>European Journal of Management and Business Economics</t>
         </is>
       </c>
       <c r="B18">
@@ -542,21 +542,21 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>European Journal of Management and Business Economics</t>
+          <t>European Journal of Marketing</t>
         </is>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>European Journal of Marketing</t>
+          <t>Evidence-based HRM a Global Forum for Empirical Scholarship</t>
         </is>
       </c>
       <c r="B20">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -582,7 +582,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Health Education</t>
+          <t>Industrial and Commercial Training</t>
         </is>
       </c>
       <c r="B23">
@@ -592,7 +592,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Industrial and Commercial Training</t>
+          <t>Industrial Lubrication and Tribology</t>
         </is>
       </c>
       <c r="B24">
@@ -602,17 +602,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Industrial Lubrication and Tribology</t>
+          <t>Industrial Management &amp; Data Systems</t>
         </is>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Industrial Management &amp; Data Systems</t>
+          <t>Industrial Robot the international journal of robotics research and application</t>
         </is>
       </c>
       <c r="B26">
@@ -622,7 +622,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Industrial Robot the international journal of robotics research and application</t>
+          <t>Info</t>
         </is>
       </c>
       <c r="B27">
@@ -632,7 +632,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Info</t>
+          <t>Information and Learning Sciences</t>
         </is>
       </c>
       <c r="B28">
@@ -642,17 +642,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Information and Learning Sciences</t>
+          <t>Interactive Technology and Smart Education</t>
         </is>
       </c>
       <c r="B29">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Information Technology and People</t>
+          <t>International Journal of Architectural Research Archnet-IJAR</t>
         </is>
       </c>
       <c r="B30">
@@ -662,17 +662,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Interactive Technology and Smart Education</t>
+          <t>International Journal of Climate Change Strategies and Management</t>
         </is>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>International Journal of Architectural Research Archnet-IJAR</t>
+          <t>International Journal of Conflict Management</t>
         </is>
       </c>
       <c r="B32">
@@ -682,67 +682,67 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>International Journal of Climate Change Strategies and Management</t>
+          <t>International Journal of Contemporary Hospitality Management</t>
         </is>
       </c>
       <c r="B33">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>International journal of comparative education and development</t>
+          <t>International Journal of Disaster Resilience in the Built Environment</t>
         </is>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>International Journal of Conflict Management</t>
+          <t>International Journal of Educational Management</t>
         </is>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>International Journal of Contemporary Hospitality Management</t>
+          <t>International Journal of Entrepreneurial Behaviour &amp; Research</t>
         </is>
       </c>
       <c r="B36">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>International Journal of Disaster Resilience in the Built Environment</t>
+          <t>International Journal of Gender and Entrepreneurship</t>
         </is>
       </c>
       <c r="B37">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>International Journal of Educational Management</t>
+          <t>International Journal of Information and Learning Technology</t>
         </is>
       </c>
       <c r="B38">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>International Journal of Entrepreneurial Behaviour &amp; Research</t>
+          <t>International Journal of Manpower</t>
         </is>
       </c>
       <c r="B39">
@@ -752,97 +752,97 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>International Journal of Gender and Entrepreneurship</t>
+          <t>International Journal of Operations &amp; Production Management</t>
         </is>
       </c>
       <c r="B40">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>International Journal of Health Care Quality Assurance</t>
+          <t>International Journal of Physical Distribution &amp; Logistics Management</t>
         </is>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>International Journal of Information and Learning Technology</t>
+          <t>International Journal of Social Economics</t>
         </is>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>International Journal of Manpower</t>
+          <t>International Journal of Sociology and Social Policy</t>
         </is>
       </c>
       <c r="B43">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>International Journal of Operations &amp; Production Management</t>
+          <t>International Journal of Sustainability in Higher Education</t>
         </is>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>International Journal of Physical Distribution &amp; Logistics Management</t>
+          <t>International Journal of Wine Business Research</t>
         </is>
       </c>
       <c r="B45">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>International Journal of Social Economics</t>
+          <t>International perspectives on inclusive education</t>
         </is>
       </c>
       <c r="B46">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>International Journal of Sociology and Social Policy</t>
+          <t>Internet Research</t>
         </is>
       </c>
       <c r="B47">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>International Journal of Sustainability in Higher Education</t>
+          <t>Journal for Multicultural Education</t>
         </is>
       </c>
       <c r="B48">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>International Journal of Wine Business Research</t>
+          <t>Journal of Aggression Conflict and Peace Research</t>
         </is>
       </c>
       <c r="B49">
@@ -852,7 +852,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>International Marketing Review</t>
+          <t>Journal of Agribusiness in Developing and Emerging Economies</t>
         </is>
       </c>
       <c r="B50">
@@ -862,7 +862,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>International perspectives on inclusive education</t>
+          <t>Journal of Business and Industrial Marketing</t>
         </is>
       </c>
       <c r="B51">
@@ -872,17 +872,17 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Internet Research</t>
+          <t>Journal of Communication Management</t>
         </is>
       </c>
       <c r="B52">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Journal for Multicultural Education</t>
+          <t>Journal of Consumer Marketing</t>
         </is>
       </c>
       <c r="B53">
@@ -892,7 +892,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Journal of Aggression Conflict and Peace Research</t>
+          <t>Journal of Documentation</t>
         </is>
       </c>
       <c r="B54">
@@ -902,27 +902,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Journal of Agribusiness in Developing and Emerging Economies</t>
+          <t>Journal of Economic Studies</t>
         </is>
       </c>
       <c r="B55">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Journal of Business and Industrial Marketing</t>
+          <t>Journal of Educational Administration</t>
         </is>
       </c>
       <c r="B56">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Journal of Communication Management</t>
+          <t>Journal of European Industrial Training</t>
         </is>
       </c>
       <c r="B57">
@@ -932,17 +932,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Journal of Consumer Marketing</t>
+          <t>Journal of Facilities Management</t>
         </is>
       </c>
       <c r="B58">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Journal of Documentation</t>
+          <t>Journal of Fashion Marketing and Management</t>
         </is>
       </c>
       <c r="B59">
@@ -952,47 +952,47 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Journal of Economic Studies</t>
+          <t>Journal of Health Organization and Management</t>
         </is>
       </c>
       <c r="B60">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Journal of Educational Administration</t>
+          <t>Journal of International Education in Business</t>
         </is>
       </c>
       <c r="B61">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Journal of European Industrial Training</t>
+          <t>Journal of Management Development</t>
         </is>
       </c>
       <c r="B62">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Journal of Facilities Management</t>
+          <t>Journal of Managerial Psychology</t>
         </is>
       </c>
       <c r="B63">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Journal of Fashion Marketing and Management</t>
+          <t>Journal of Manufacturing Technology Management</t>
         </is>
       </c>
       <c r="B64">
@@ -1002,17 +1002,17 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Journal of Health Organization and Management</t>
+          <t>Journal of Organizational Change Management</t>
         </is>
       </c>
       <c r="B65">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Journal of International Education in Business</t>
+          <t>Journal of service management</t>
         </is>
       </c>
       <c r="B66">
@@ -1022,7 +1022,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Journal of Knowledge Management</t>
+          <t>Journal of Services Marketing</t>
         </is>
       </c>
       <c r="B67">
@@ -1032,27 +1032,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Journal of Management Development</t>
+          <t>Journal of Small Business and Enterprise Development</t>
         </is>
       </c>
       <c r="B68">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Journal of Managerial Psychology</t>
+          <t>Journal of Tourism Futures</t>
         </is>
       </c>
       <c r="B69">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Journal of Manufacturing Technology Management</t>
+          <t>Journal of Workplace Learning</t>
         </is>
       </c>
       <c r="B70">
@@ -1062,27 +1062,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Journal of Organizational Change Management</t>
+          <t>Kybernetes</t>
         </is>
       </c>
       <c r="B71">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Journal of Product &amp; Brand Management</t>
+          <t>Leadership &amp; Organization Development Journal</t>
         </is>
       </c>
       <c r="B72">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Journal of Research in Interactive Marketing</t>
+          <t>Library Hi Tech</t>
         </is>
       </c>
       <c r="B73">
@@ -1092,17 +1092,17 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Journal of service management</t>
+          <t>Library Management</t>
         </is>
       </c>
       <c r="B74">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Journal of Small Business and Enterprise Development</t>
+          <t>Library Review</t>
         </is>
       </c>
       <c r="B75">
@@ -1112,7 +1112,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Journal of Tourism Futures</t>
+          <t>Literacy research, practice and evaluation</t>
         </is>
       </c>
       <c r="B76">
@@ -1122,27 +1122,27 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Kybernetes</t>
+          <t>Management Decision</t>
         </is>
       </c>
       <c r="B77">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Leadership &amp; Organization Development Journal</t>
+          <t>Management of Environmental Quality An International Journal</t>
         </is>
       </c>
       <c r="B78">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Library Hi Tech</t>
+          <t>Management Research News</t>
         </is>
       </c>
       <c r="B79">
@@ -1152,7 +1152,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Library Management</t>
+          <t>Managing Service Quality</t>
         </is>
       </c>
       <c r="B80">
@@ -1162,17 +1162,17 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Library Review</t>
+          <t>Microelectronics International</t>
         </is>
       </c>
       <c r="B81">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Literacy research, practice and evaluation</t>
+          <t>New England journal of entrepreneurship</t>
         </is>
       </c>
       <c r="B82">
@@ -1182,7 +1182,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Management Decision</t>
+          <t>Nutrition &amp; Food Science</t>
         </is>
       </c>
       <c r="B83">
@@ -1192,17 +1192,17 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Management of Environmental Quality An International Journal</t>
+          <t>On the Horizon The International Journal of Learning Futures</t>
         </is>
       </c>
       <c r="B84">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Management Research News</t>
+          <t>Organization Management Journal</t>
         </is>
       </c>
       <c r="B85">
@@ -1212,47 +1212,47 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Managing Service Quality</t>
+          <t>Personnel Review</t>
         </is>
       </c>
       <c r="B86">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Microelectronics International</t>
+          <t>Policing An International Journal</t>
         </is>
       </c>
       <c r="B87">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>New England journal of entrepreneurship</t>
+          <t>Qualitative Market Research An International Journal</t>
         </is>
       </c>
       <c r="B88">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Nutrition &amp; Food Science</t>
+          <t>Qualitative Research in Accounting &amp; Management</t>
         </is>
       </c>
       <c r="B89">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>On the Horizon The International Journal of Learning Futures</t>
+          <t>Qualitative Research in Organizations and Management An International Journal</t>
         </is>
       </c>
       <c r="B90">
@@ -1262,37 +1262,37 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Personnel Review</t>
+          <t>Rapid Prototyping Journal</t>
         </is>
       </c>
       <c r="B91">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Policing An International Journal</t>
+          <t>Reference Reviews</t>
         </is>
       </c>
       <c r="B92">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Qualitative Market Research An International Journal</t>
+          <t>Reference Services Review</t>
         </is>
       </c>
       <c r="B93">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Qualitative Research in Accounting &amp; Management</t>
+          <t>Research in community and mental health</t>
         </is>
       </c>
       <c r="B94">
@@ -1302,47 +1302,47 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Qualitative Research Journal</t>
+          <t>Research in experimental economics</t>
         </is>
       </c>
       <c r="B95">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Rapid Prototyping Journal</t>
+          <t>Research in social movements, conflicts and change</t>
         </is>
       </c>
       <c r="B96">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Reference Reviews</t>
+          <t>Research in social problems and public policy</t>
         </is>
       </c>
       <c r="B97">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Reference Services Review</t>
+          <t>Research in the history of economic thought and methodology</t>
         </is>
       </c>
       <c r="B98">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Research in community and mental health</t>
+          <t>Research in the sociology of health care</t>
         </is>
       </c>
       <c r="B99">
@@ -1352,57 +1352,57 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Research in experimental economics</t>
+          <t>Research in the sociology of organizations</t>
         </is>
       </c>
       <c r="B100">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Research in social movements, conflicts and change</t>
+          <t>Review of Accounting and Finance</t>
         </is>
       </c>
       <c r="B101">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Research in social problems and public policy</t>
+          <t>Review of marketing research</t>
         </is>
       </c>
       <c r="B102">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Research in the sociology of health care</t>
+          <t>Sensor Review</t>
         </is>
       </c>
       <c r="B103">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Research in the sociology of organizations</t>
+          <t>Smart and Sustainable Built Environment</t>
         </is>
       </c>
       <c r="B104">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Review of Accounting and Finance</t>
+          <t>Social Responsibility Journal</t>
         </is>
       </c>
       <c r="B105">
@@ -1412,7 +1412,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Review of marketing research</t>
+          <t>Society and Business Review</t>
         </is>
       </c>
       <c r="B106">
@@ -1422,27 +1422,27 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Sensor Review</t>
+          <t>Strategic HR Review</t>
         </is>
       </c>
       <c r="B107">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Smart and Sustainable Built Environment</t>
+          <t>Strategy and Leadership</t>
         </is>
       </c>
       <c r="B108">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Social Responsibility Journal</t>
+          <t>Studies in Economics and Finance</t>
         </is>
       </c>
       <c r="B109">
@@ -1452,27 +1452,27 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Society and Business Review</t>
+          <t>Studies in media and communications</t>
         </is>
       </c>
       <c r="B110">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Strategic Direction</t>
+          <t>Technology, innovation, entrepreneurship and competitive strategy</t>
         </is>
       </c>
       <c r="B111">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Strategic HR Review</t>
+          <t>The Electronic Library</t>
         </is>
       </c>
       <c r="B112">
@@ -1482,27 +1482,27 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Strategy and Leadership</t>
+          <t>Tizard Learning Disability Review</t>
         </is>
       </c>
       <c r="B113">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Studies in media and communications</t>
+          <t>VINE</t>
         </is>
       </c>
       <c r="B114">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Supply Chain Management An International Journal</t>
+          <t>Work Study</t>
         </is>
       </c>
       <c r="B115">
@@ -1512,60 +1512,10 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Technology, innovation, entrepreneurship and competitive strategy</t>
+          <t>Young Consumers Insight and Ideas for Responsible Marketers</t>
         </is>
       </c>
       <c r="B116">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>The Electronic Library</t>
-        </is>
-      </c>
-      <c r="B117">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>Tizard Learning Disability Review</t>
-        </is>
-      </c>
-      <c r="B118">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="inlineStr">
-        <is>
-          <t>VINE</t>
-        </is>
-      </c>
-      <c r="B119">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="inlineStr">
-        <is>
-          <t>Work Study</t>
-        </is>
-      </c>
-      <c r="B120">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="inlineStr">
-        <is>
-          <t>Young Consumers Insight and Ideas for Responsible Marketers</t>
-        </is>
-      </c>
-      <c r="B121">
         <v>2</v>
       </c>
     </row>

</xml_diff>